<commit_message>
update excel test data and file run_test_scripts.sh
</commit_message>
<xml_diff>
--- a/test-project-web-robotframework/resouces/testdata/testdata_shp.xlsx
+++ b/test-project-web-robotframework/resouces/testdata/testdata_shp.xlsx
@@ -73,10 +73,10 @@
     <t>SHP-0001-TD-003</t>
   </si>
   <si>
-    <t>นินจาคาถา โอ้โฮเฮะ เล่ม 23</t>
-  </si>
-  <si>
-    <t>นินจาคาถา โอ้โฮเฮะ เล่ม 66</t>
+    <t>มหาศึกคนชนคน เล่ม 1</t>
+  </si>
+  <si>
+    <t>มหาศึกคนชนคน เล่ม 2</t>
   </si>
 </sst>
 </file>
@@ -721,7 +721,7 @@
       <c r="E11" s="15"/>
       <c r="F11" s="16"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="21">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="15"/>
       <c r="B12" s="15"/>
       <c r="C12" s="15"/>

</xml_diff>